<commit_message>
-Updated Excels images and fix bug in experimento 1
</commit_message>
<xml_diff>
--- a/Resultados/Experimento1/tabla_metricas.xlsx
+++ b/Resultados/Experimento1/tabla_metricas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS22"/>
+  <dimension ref="A1:AO21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,160 +501,140 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Exactitud Random Ciclico</t>
+          <t>Exactitud Random Ciclico Extended</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Precision Random Ciclico</t>
+          <t>Precision Random Ciclico Extended</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Sensibilidad Random Ciclico</t>
+          <t>Sensibilidad Random Ciclico Extended</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>F1 Score Random Ciclico</t>
+          <t>F1 Score Random Ciclico Extended</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Exactitud Random Ciclico Extended</t>
+          <t>Exactitud Ciclico</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Precision Random Ciclico Extended</t>
+          <t>Precision Ciclico</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Sensibilidad Random Ciclico Extended</t>
+          <t>Sensibilidad Ciclico</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>F1 Score Random Ciclico Extended</t>
+          <t>F1 Score Ciclico</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Exactitud Ciclico</t>
+          <t>Exactitud LBFGS</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Precision Ciclico</t>
+          <t>Precision LBFGS</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Sensibilidad Ciclico</t>
+          <t>Sensibilidad LBFGS</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>F1 Score Ciclico</t>
+          <t>F1 Score LBFGS</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Exactitud LBFGS</t>
+          <t>Exactitud Fijo</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Precision LBFGS</t>
+          <t>Precision Fijo</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Sensibilidad LBFGS</t>
+          <t>Sensibilidad Fijo</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>F1 Score LBFGS</t>
+          <t>F1 Score Fijo</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>Exactitud Fijo</t>
+          <t>Exactitud Adam</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>Precision Fijo</t>
+          <t>Precision Adam</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>Sensibilidad Fijo</t>
+          <t>Sensibilidad Adam</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>F1 Score Fijo</t>
+          <t>F1 Score Adam</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>Exactitud Adam</t>
+          <t>Exactitud Decreciente</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>Precision Adam</t>
+          <t>Precision Decreciente</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>Sensibilidad Adam</t>
+          <t>Sensibilidad Decreciente</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>F1 Score Adam</t>
+          <t>F1 Score Decreciente</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>Exactitud Decreciente</t>
+          <t>Exactitud LBFGS_LS</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>Precision Decreciente</t>
+          <t>Precision LBFGS_LS</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>Sensibilidad Decreciente</t>
+          <t>Sensibilidad LBFGS_LS</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>F1 Score Decreciente</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>Exactitud LBFGS_LS</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>Precision LBFGS_LS</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>Sensibilidad LBFGS_LS</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>F1 Score LBFGS_LS</t>
         </is>
@@ -689,112 +669,100 @@
         <v>98.68000000000001</v>
       </c>
       <c r="J2" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
       </c>
       <c r="K2" t="n">
-        <v>98.28</v>
+        <v>98.33</v>
       </c>
       <c r="L2" t="n">
-        <v>99.13</v>
+        <v>99.16</v>
       </c>
       <c r="M2" t="n">
-        <v>98.7</v>
+        <v>98.73999999999999</v>
       </c>
       <c r="N2" t="n">
         <v>98.29000000000001</v>
       </c>
       <c r="O2" t="n">
-        <v>98.08</v>
+        <v>98.39</v>
       </c>
       <c r="P2" t="n">
-        <v>99.06999999999999</v>
+        <v>99.09</v>
       </c>
       <c r="Q2" t="n">
-        <v>98.58</v>
+        <v>98.73999999999999</v>
       </c>
       <c r="R2" t="n">
-        <v>98.29000000000001</v>
+        <v>98.28</v>
       </c>
       <c r="S2" t="n">
-        <v>98.39</v>
+        <v>98.20999999999999</v>
       </c>
       <c r="T2" t="n">
-        <v>99.09</v>
+        <v>99.12</v>
       </c>
       <c r="U2" t="n">
-        <v>98.73999999999999</v>
+        <v>98.67</v>
       </c>
       <c r="V2" t="n">
-        <v>98.28</v>
+        <v>98.06999999999999</v>
       </c>
       <c r="W2" t="n">
-        <v>98.20999999999999</v>
+        <v>98.44</v>
       </c>
       <c r="X2" t="n">
-        <v>99.12</v>
+        <v>98.95999999999999</v>
       </c>
       <c r="Y2" t="n">
-        <v>98.67</v>
+        <v>98.7</v>
       </c>
       <c r="Z2" t="n">
-        <v>98.06999999999999</v>
+        <v>97.91</v>
       </c>
       <c r="AA2" t="n">
-        <v>98.44</v>
+        <v>98.33</v>
       </c>
       <c r="AB2" t="n">
-        <v>98.95999999999999</v>
+        <v>98.78</v>
       </c>
       <c r="AC2" t="n">
+        <v>98.55</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>97.02</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>97.06999999999999</v>
+      </c>
+      <c r="AF2" t="n">
         <v>98.7</v>
       </c>
-      <c r="AD2" t="n">
-        <v>97.91</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>98.33</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>98.78</v>
-      </c>
       <c r="AG2" t="n">
-        <v>98.55</v>
+        <v>97.88</v>
       </c>
       <c r="AH2" t="n">
-        <v>97.02</v>
+        <v>96.84999999999999</v>
       </c>
       <c r="AI2" t="n">
-        <v>97.06999999999999</v>
+        <v>98.43000000000001</v>
       </c>
       <c r="AJ2" t="n">
-        <v>98.7</v>
+        <v>98.31999999999999</v>
       </c>
       <c r="AK2" t="n">
-        <v>97.88</v>
+        <v>98.37</v>
       </c>
       <c r="AL2" t="n">
-        <v>96.84999999999999</v>
+        <v>98.37</v>
       </c>
       <c r="AM2" t="n">
         <v>98.43000000000001</v>
       </c>
       <c r="AN2" t="n">
-        <v>98.31999999999999</v>
+        <v>99.09999999999999</v>
       </c>
       <c r="AO2" t="n">
-        <v>98.37</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>94.3</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>95.22</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>98.39</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>96.78</v>
+        <v>98.76000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -826,112 +794,100 @@
         <v>99.19</v>
       </c>
       <c r="J3" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
       </c>
       <c r="K3" t="n">
-        <v>99.09999999999999</v>
+        <v>99.12</v>
       </c>
       <c r="L3" t="n">
-        <v>99.27</v>
+        <v>99.29000000000001</v>
       </c>
       <c r="M3" t="n">
-        <v>99.18000000000001</v>
+        <v>99.2</v>
       </c>
       <c r="N3" t="n">
         <v>98.29000000000001</v>
       </c>
       <c r="O3" t="n">
-        <v>99.12</v>
+        <v>99.02</v>
       </c>
       <c r="P3" t="n">
+        <v>99.28</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>99.15000000000001</v>
+      </c>
+      <c r="R3" t="n">
+        <v>98.28</v>
+      </c>
+      <c r="S3" t="n">
+        <v>99.06</v>
+      </c>
+      <c r="T3" t="n">
+        <v>99.27</v>
+      </c>
+      <c r="U3" t="n">
+        <v>99.16</v>
+      </c>
+      <c r="V3" t="n">
+        <v>98.06999999999999</v>
+      </c>
+      <c r="W3" t="n">
+        <v>99.14</v>
+      </c>
+      <c r="X3" t="n">
+        <v>99.34</v>
+      </c>
+      <c r="Y3" t="n">
         <v>99.23999999999999</v>
       </c>
-      <c r="Q3" t="n">
-        <v>99.18000000000001</v>
-      </c>
-      <c r="R3" t="n">
-        <v>98.29000000000001</v>
-      </c>
-      <c r="S3" t="n">
-        <v>99.02</v>
-      </c>
-      <c r="T3" t="n">
-        <v>99.28</v>
-      </c>
-      <c r="U3" t="n">
-        <v>99.15000000000001</v>
-      </c>
-      <c r="V3" t="n">
+      <c r="Z3" t="n">
+        <v>97.91</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>99.04000000000001</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>99.14</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>99.09</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>97.02</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>98.03</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>98.89</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>98.45999999999999</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>96.84999999999999</v>
+      </c>
+      <c r="AI3" t="n">
         <v>98.28</v>
       </c>
-      <c r="W3" t="n">
+      <c r="AJ3" t="n">
+        <v>98.48999999999999</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>98.39</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>98.37</v>
+      </c>
+      <c r="AM3" t="n">
         <v>99.06</v>
       </c>
-      <c r="X3" t="n">
-        <v>99.27</v>
-      </c>
-      <c r="Y3" t="n">
+      <c r="AN3" t="n">
+        <v>99.25</v>
+      </c>
+      <c r="AO3" t="n">
         <v>99.16</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>98.06999999999999</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>99.14</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>99.34</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>99.23999999999999</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>97.91</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>99.04000000000001</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>99.14</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>99.09</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>97.02</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>98.03</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>98.89</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>98.45999999999999</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>96.84999999999999</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>98.28</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>98.48999999999999</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>98.39</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>94.3</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>97.11</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>98.16</v>
-      </c>
-      <c r="AS3" t="n">
-        <v>97.63</v>
       </c>
     </row>
     <row r="4">
@@ -963,112 +919,100 @@
         <v>98.33</v>
       </c>
       <c r="J4" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
       </c>
       <c r="K4" t="n">
-        <v>98.26000000000001</v>
+        <v>98.33</v>
       </c>
       <c r="L4" t="n">
-        <v>98.36</v>
+        <v>98.42</v>
       </c>
       <c r="M4" t="n">
-        <v>98.31</v>
+        <v>98.38</v>
       </c>
       <c r="N4" t="n">
         <v>98.29000000000001</v>
       </c>
       <c r="O4" t="n">
+        <v>98.01000000000001</v>
+      </c>
+      <c r="P4" t="n">
+        <v>98.42</v>
+      </c>
+      <c r="Q4" t="n">
         <v>98.20999999999999</v>
       </c>
-      <c r="P4" t="n">
-        <v>98.31999999999999</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>98.27</v>
-      </c>
       <c r="R4" t="n">
+        <v>98.28</v>
+      </c>
+      <c r="S4" t="n">
+        <v>98.09</v>
+      </c>
+      <c r="T4" t="n">
+        <v>98.31</v>
+      </c>
+      <c r="U4" t="n">
+        <v>98.2</v>
+      </c>
+      <c r="V4" t="n">
+        <v>98.06999999999999</v>
+      </c>
+      <c r="W4" t="n">
+        <v>97.97</v>
+      </c>
+      <c r="X4" t="n">
+        <v>97.86</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>97.91</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>97.91</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>97.84</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>97.90000000000001</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>97.87</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>97.02</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>97.19</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>97.03</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>97.11</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>96.84999999999999</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>96.7</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>97.2</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>96.95</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>98.37</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>98.18000000000001</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>98.41</v>
+      </c>
+      <c r="AO4" t="n">
         <v>98.29000000000001</v>
-      </c>
-      <c r="S4" t="n">
-        <v>98.01000000000001</v>
-      </c>
-      <c r="T4" t="n">
-        <v>98.42</v>
-      </c>
-      <c r="U4" t="n">
-        <v>98.20999999999999</v>
-      </c>
-      <c r="V4" t="n">
-        <v>98.28</v>
-      </c>
-      <c r="W4" t="n">
-        <v>98.09</v>
-      </c>
-      <c r="X4" t="n">
-        <v>98.31</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>98.2</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>98.06999999999999</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>97.97</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>97.86</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>97.91</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>97.91</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>97.84</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>97.90000000000001</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>97.87</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>97.02</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>97.19</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>97.03</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>97.11</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>96.84999999999999</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>96.7</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>97.2</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>96.95</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>94.3</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>94.72</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>93.09</v>
-      </c>
-      <c r="AS4" t="n">
-        <v>93.90000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -1100,112 +1044,100 @@
         <v>98.22</v>
       </c>
       <c r="J5" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
       </c>
       <c r="K5" t="n">
-        <v>98</v>
+        <v>98.20999999999999</v>
       </c>
       <c r="L5" t="n">
-        <v>98.45999999999999</v>
+        <v>98.31</v>
       </c>
       <c r="M5" t="n">
-        <v>98.23</v>
+        <v>98.26000000000001</v>
       </c>
       <c r="N5" t="n">
         <v>98.29000000000001</v>
       </c>
       <c r="O5" t="n">
-        <v>98.03</v>
+        <v>98.05</v>
       </c>
       <c r="P5" t="n">
-        <v>98.34999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="Q5" t="n">
-        <v>98.19</v>
+        <v>98.22</v>
       </c>
       <c r="R5" t="n">
-        <v>98.29000000000001</v>
+        <v>98.28</v>
       </c>
       <c r="S5" t="n">
-        <v>98.05</v>
+        <v>98.02</v>
       </c>
       <c r="T5" t="n">
+        <v>98.26000000000001</v>
+      </c>
+      <c r="U5" t="n">
+        <v>98.14</v>
+      </c>
+      <c r="V5" t="n">
+        <v>98.06999999999999</v>
+      </c>
+      <c r="W5" t="n">
+        <v>97.3</v>
+      </c>
+      <c r="X5" t="n">
+        <v>98.06999999999999</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>97.69</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>97.91</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>97.31</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>97.56999999999999</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>97.44</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>97.02</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>96.33</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>97.33</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>96.83</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>96.84999999999999</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>96.37</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>96.65000000000001</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>96.51000000000001</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>98.37</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>98.14</v>
+      </c>
+      <c r="AN5" t="n">
         <v>98.40000000000001</v>
       </c>
-      <c r="U5" t="n">
-        <v>98.22</v>
-      </c>
-      <c r="V5" t="n">
-        <v>98.28</v>
-      </c>
-      <c r="W5" t="n">
-        <v>98.02</v>
-      </c>
-      <c r="X5" t="n">
-        <v>98.26000000000001</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>98.14</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>98.06999999999999</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>97.3</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>98.06999999999999</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>97.69</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>97.91</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>97.31</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>97.56999999999999</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>97.44</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>97.02</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>96.33</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>97.33</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>96.83</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>96.84999999999999</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>96.37</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>96.65000000000001</v>
-      </c>
       <c r="AO5" t="n">
-        <v>96.51000000000001</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>94.3</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>92.70999999999999</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>94.16</v>
-      </c>
-      <c r="AS5" t="n">
-        <v>93.43000000000001</v>
+        <v>98.27</v>
       </c>
     </row>
     <row r="6">
@@ -1237,112 +1169,100 @@
         <v>98.34</v>
       </c>
       <c r="J6" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
       </c>
       <c r="K6" t="n">
-        <v>98.45999999999999</v>
+        <v>98.42</v>
       </c>
       <c r="L6" t="n">
-        <v>98.25</v>
+        <v>98.31999999999999</v>
       </c>
       <c r="M6" t="n">
-        <v>98.34999999999999</v>
+        <v>98.37</v>
       </c>
       <c r="N6" t="n">
         <v>98.29000000000001</v>
       </c>
       <c r="O6" t="n">
-        <v>98.48999999999999</v>
+        <v>98.44</v>
       </c>
       <c r="P6" t="n">
-        <v>98.02</v>
+        <v>98.08</v>
       </c>
       <c r="Q6" t="n">
-        <v>98.25</v>
+        <v>98.26000000000001</v>
       </c>
       <c r="R6" t="n">
+        <v>98.28</v>
+      </c>
+      <c r="S6" t="n">
+        <v>98.36</v>
+      </c>
+      <c r="T6" t="n">
+        <v>98.18000000000001</v>
+      </c>
+      <c r="U6" t="n">
+        <v>98.27</v>
+      </c>
+      <c r="V6" t="n">
+        <v>98.06999999999999</v>
+      </c>
+      <c r="W6" t="n">
+        <v>98.17</v>
+      </c>
+      <c r="X6" t="n">
+        <v>97.83</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>98</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>97.91</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>98.43000000000001</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>97.64</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>98.04000000000001</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>97.02</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>96.90000000000001</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>97.11</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>97.01000000000001</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>96.84999999999999</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>97.08</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>96.90000000000001</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>96.98999999999999</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>98.37</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>98.31</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>98.28</v>
+      </c>
+      <c r="AO6" t="n">
         <v>98.29000000000001</v>
-      </c>
-      <c r="S6" t="n">
-        <v>98.44</v>
-      </c>
-      <c r="T6" t="n">
-        <v>98.08</v>
-      </c>
-      <c r="U6" t="n">
-        <v>98.26000000000001</v>
-      </c>
-      <c r="V6" t="n">
-        <v>98.28</v>
-      </c>
-      <c r="W6" t="n">
-        <v>98.36</v>
-      </c>
-      <c r="X6" t="n">
-        <v>98.18000000000001</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>98.27</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>98.06999999999999</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>98.17</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>97.83</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>98</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>97.91</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>98.43000000000001</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>97.64</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>98.04000000000001</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>97.02</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>96.90000000000001</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>97.11</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>97.01000000000001</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>96.84999999999999</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>97.08</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>96.90000000000001</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>96.98999999999999</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>94.3</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>93.22</v>
-      </c>
-      <c r="AR6" t="n">
-        <v>94.91</v>
-      </c>
-      <c r="AS6" t="n">
-        <v>94.06</v>
       </c>
     </row>
     <row r="7">
@@ -1374,112 +1294,100 @@
         <v>98.3</v>
       </c>
       <c r="J7" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
       </c>
       <c r="K7" t="n">
-        <v>98.61</v>
+        <v>98.64</v>
       </c>
       <c r="L7" t="n">
-        <v>97.84</v>
+        <v>97.93000000000001</v>
       </c>
       <c r="M7" t="n">
-        <v>98.23</v>
+        <v>98.28</v>
       </c>
       <c r="N7" t="n">
         <v>98.29000000000001</v>
       </c>
       <c r="O7" t="n">
-        <v>98.58</v>
+        <v>98.75</v>
       </c>
       <c r="P7" t="n">
-        <v>97.93000000000001</v>
+        <v>97.73999999999999</v>
       </c>
       <c r="Q7" t="n">
-        <v>98.25</v>
+        <v>98.23999999999999</v>
       </c>
       <c r="R7" t="n">
-        <v>98.29000000000001</v>
+        <v>98.28</v>
       </c>
       <c r="S7" t="n">
-        <v>98.75</v>
+        <v>98.62</v>
       </c>
       <c r="T7" t="n">
-        <v>97.73999999999999</v>
+        <v>97.8</v>
       </c>
       <c r="U7" t="n">
-        <v>98.23999999999999</v>
+        <v>98.20999999999999</v>
       </c>
       <c r="V7" t="n">
+        <v>98.06999999999999</v>
+      </c>
+      <c r="W7" t="n">
+        <v>98.26000000000001</v>
+      </c>
+      <c r="X7" t="n">
+        <v>97.33</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>97.79000000000001</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>97.91</v>
+      </c>
+      <c r="AA7" t="n">
         <v>98.28</v>
       </c>
-      <c r="W7" t="n">
-        <v>98.62</v>
-      </c>
-      <c r="X7" t="n">
-        <v>97.8</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>98.20999999999999</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>98.06999999999999</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>98.26000000000001</v>
-      </c>
       <c r="AB7" t="n">
-        <v>97.33</v>
+        <v>97.23</v>
       </c>
       <c r="AC7" t="n">
-        <v>97.79000000000001</v>
+        <v>97.75</v>
       </c>
       <c r="AD7" t="n">
-        <v>97.91</v>
+        <v>97.02</v>
       </c>
       <c r="AE7" t="n">
-        <v>98.28</v>
+        <v>97.37</v>
       </c>
       <c r="AF7" t="n">
-        <v>97.23</v>
+        <v>96</v>
       </c>
       <c r="AG7" t="n">
-        <v>97.75</v>
+        <v>96.68000000000001</v>
       </c>
       <c r="AH7" t="n">
-        <v>97.02</v>
+        <v>96.84999999999999</v>
       </c>
       <c r="AI7" t="n">
-        <v>97.37</v>
+        <v>95.5</v>
       </c>
       <c r="AJ7" t="n">
-        <v>96</v>
+        <v>96.43000000000001</v>
       </c>
       <c r="AK7" t="n">
-        <v>96.68000000000001</v>
+        <v>95.97</v>
       </c>
       <c r="AL7" t="n">
-        <v>96.84999999999999</v>
+        <v>98.37</v>
       </c>
       <c r="AM7" t="n">
-        <v>95.5</v>
+        <v>98.67</v>
       </c>
       <c r="AN7" t="n">
-        <v>96.43000000000001</v>
+        <v>97.98999999999999</v>
       </c>
       <c r="AO7" t="n">
-        <v>95.97</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>94.3</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>94.43000000000001</v>
-      </c>
-      <c r="AR7" t="n">
-        <v>90.73</v>
-      </c>
-      <c r="AS7" t="n">
-        <v>92.54000000000001</v>
+        <v>98.33</v>
       </c>
     </row>
     <row r="8">
@@ -1511,112 +1419,100 @@
         <v>98.48999999999999</v>
       </c>
       <c r="J8" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
       </c>
       <c r="K8" t="n">
-        <v>98.31</v>
+        <v>98.23999999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>98.59</v>
+        <v>98.59999999999999</v>
       </c>
       <c r="M8" t="n">
-        <v>98.45</v>
+        <v>98.42</v>
       </c>
       <c r="N8" t="n">
         <v>98.29000000000001</v>
       </c>
       <c r="O8" t="n">
-        <v>98.29000000000001</v>
+        <v>98.16</v>
       </c>
       <c r="P8" t="n">
-        <v>98.45999999999999</v>
+        <v>98.5</v>
       </c>
       <c r="Q8" t="n">
-        <v>98.38</v>
+        <v>98.33</v>
       </c>
       <c r="R8" t="n">
-        <v>98.29000000000001</v>
+        <v>98.28</v>
       </c>
       <c r="S8" t="n">
-        <v>98.16</v>
+        <v>98.23999999999999</v>
       </c>
       <c r="T8" t="n">
-        <v>98.5</v>
+        <v>98.51000000000001</v>
       </c>
       <c r="U8" t="n">
+        <v>98.37</v>
+      </c>
+      <c r="V8" t="n">
+        <v>98.06999999999999</v>
+      </c>
+      <c r="W8" t="n">
+        <v>98.27</v>
+      </c>
+      <c r="X8" t="n">
+        <v>98.2</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>98.23999999999999</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>97.91</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>97.94</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>98.42</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>98.18000000000001</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>97.02</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>96.81999999999999</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>97.16</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>96.98999999999999</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>96.84999999999999</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>97.56</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>97.23</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>97.39</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>98.37</v>
+      </c>
+      <c r="AM8" t="n">
         <v>98.33</v>
       </c>
-      <c r="V8" t="n">
-        <v>98.28</v>
-      </c>
-      <c r="W8" t="n">
-        <v>98.23999999999999</v>
-      </c>
-      <c r="X8" t="n">
-        <v>98.51000000000001</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>98.37</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>98.06999999999999</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>98.27</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>98.2</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>98.23999999999999</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>97.91</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>97.94</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>98.42</v>
-      </c>
-      <c r="AG8" t="n">
-        <v>98.18000000000001</v>
-      </c>
-      <c r="AH8" t="n">
-        <v>97.02</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>96.81999999999999</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>97.16</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>96.98999999999999</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>96.84999999999999</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>97.56</v>
-      </c>
       <c r="AN8" t="n">
-        <v>97.23</v>
+        <v>98.53</v>
       </c>
       <c r="AO8" t="n">
-        <v>97.39</v>
-      </c>
-      <c r="AP8" t="n">
-        <v>94.3</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>93.76000000000001</v>
-      </c>
-      <c r="AR8" t="n">
-        <v>95.98999999999999</v>
-      </c>
-      <c r="AS8" t="n">
-        <v>94.86</v>
+        <v>98.43000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -1648,112 +1544,100 @@
         <v>97.98999999999999</v>
       </c>
       <c r="J9" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
       </c>
       <c r="K9" t="n">
-        <v>97.95999999999999</v>
+        <v>97.91</v>
       </c>
       <c r="L9" t="n">
         <v>98.02</v>
       </c>
       <c r="M9" t="n">
-        <v>97.98999999999999</v>
+        <v>97.95999999999999</v>
       </c>
       <c r="N9" t="n">
         <v>98.29000000000001</v>
       </c>
       <c r="O9" t="n">
+        <v>98.01000000000001</v>
+      </c>
+      <c r="P9" t="n">
+        <v>97.75</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>97.88</v>
+      </c>
+      <c r="R9" t="n">
+        <v>98.28</v>
+      </c>
+      <c r="S9" t="n">
+        <v>97.94</v>
+      </c>
+      <c r="T9" t="n">
+        <v>97.83</v>
+      </c>
+      <c r="U9" t="n">
+        <v>97.89</v>
+      </c>
+      <c r="V9" t="n">
+        <v>98.06999999999999</v>
+      </c>
+      <c r="W9" t="n">
+        <v>98.04000000000001</v>
+      </c>
+      <c r="X9" t="n">
         <v>97.95999999999999</v>
       </c>
-      <c r="P9" t="n">
-        <v>97.87</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>97.92</v>
-      </c>
-      <c r="R9" t="n">
-        <v>98.29000000000001</v>
-      </c>
-      <c r="S9" t="n">
-        <v>98.01000000000001</v>
-      </c>
-      <c r="T9" t="n">
-        <v>97.75</v>
-      </c>
-      <c r="U9" t="n">
-        <v>97.88</v>
-      </c>
-      <c r="V9" t="n">
-        <v>98.28</v>
-      </c>
-      <c r="W9" t="n">
-        <v>97.94</v>
-      </c>
-      <c r="X9" t="n">
-        <v>97.83</v>
-      </c>
       <c r="Y9" t="n">
-        <v>97.89</v>
+        <v>98</v>
       </c>
       <c r="Z9" t="n">
-        <v>98.06999999999999</v>
+        <v>97.91</v>
       </c>
       <c r="AA9" t="n">
-        <v>98.04000000000001</v>
+        <v>97.8</v>
       </c>
       <c r="AB9" t="n">
-        <v>97.95999999999999</v>
+        <v>97.64</v>
       </c>
       <c r="AC9" t="n">
-        <v>98</v>
+        <v>97.72</v>
       </c>
       <c r="AD9" t="n">
+        <v>97.02</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>96.56999999999999</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>96.48</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>96.52</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>96.84999999999999</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>97.48</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>96.44</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>96.95999999999999</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>98.37</v>
+      </c>
+      <c r="AM9" t="n">
         <v>97.91</v>
       </c>
-      <c r="AE9" t="n">
-        <v>97.8</v>
-      </c>
-      <c r="AF9" t="n">
-        <v>97.64</v>
-      </c>
-      <c r="AG9" t="n">
-        <v>97.72</v>
-      </c>
-      <c r="AH9" t="n">
-        <v>97.02</v>
-      </c>
-      <c r="AI9" t="n">
-        <v>96.56999999999999</v>
-      </c>
-      <c r="AJ9" t="n">
-        <v>96.48</v>
-      </c>
-      <c r="AK9" t="n">
-        <v>96.52</v>
-      </c>
-      <c r="AL9" t="n">
-        <v>96.84999999999999</v>
-      </c>
-      <c r="AM9" t="n">
-        <v>97.48</v>
-      </c>
       <c r="AN9" t="n">
-        <v>96.44</v>
+        <v>98.02</v>
       </c>
       <c r="AO9" t="n">
-        <v>96.95999999999999</v>
-      </c>
-      <c r="AP9" t="n">
-        <v>94.3</v>
-      </c>
-      <c r="AQ9" t="n">
-        <v>94.7</v>
-      </c>
-      <c r="AR9" t="n">
-        <v>93.56999999999999</v>
-      </c>
-      <c r="AS9" t="n">
-        <v>94.13</v>
+        <v>97.97</v>
       </c>
     </row>
     <row r="10">
@@ -1785,112 +1669,100 @@
         <v>98.2</v>
       </c>
       <c r="J10" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
       </c>
       <c r="K10" t="n">
-        <v>98.54000000000001</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="L10" t="n">
-        <v>97.83</v>
+        <v>97.89</v>
       </c>
       <c r="M10" t="n">
-        <v>98.18000000000001</v>
+        <v>98.14</v>
       </c>
       <c r="N10" t="n">
         <v>98.29000000000001</v>
       </c>
       <c r="O10" t="n">
-        <v>98.27</v>
+        <v>98.23</v>
       </c>
       <c r="P10" t="n">
-        <v>97.8</v>
+        <v>97.84</v>
       </c>
       <c r="Q10" t="n">
         <v>98.04000000000001</v>
       </c>
       <c r="R10" t="n">
+        <v>98.28</v>
+      </c>
+      <c r="S10" t="n">
         <v>98.29000000000001</v>
       </c>
-      <c r="S10" t="n">
-        <v>98.23</v>
-      </c>
       <c r="T10" t="n">
-        <v>97.84</v>
+        <v>97.8</v>
       </c>
       <c r="U10" t="n">
         <v>98.04000000000001</v>
       </c>
       <c r="V10" t="n">
-        <v>98.28</v>
+        <v>98.06999999999999</v>
       </c>
       <c r="W10" t="n">
-        <v>98.29000000000001</v>
+        <v>97.72</v>
       </c>
       <c r="X10" t="n">
-        <v>97.8</v>
+        <v>97.59</v>
       </c>
       <c r="Y10" t="n">
-        <v>98.04000000000001</v>
+        <v>97.66</v>
       </c>
       <c r="Z10" t="n">
-        <v>98.06999999999999</v>
+        <v>97.91</v>
       </c>
       <c r="AA10" t="n">
-        <v>97.72</v>
+        <v>97.08</v>
       </c>
       <c r="AB10" t="n">
-        <v>97.59</v>
+        <v>97.39</v>
       </c>
       <c r="AC10" t="n">
-        <v>97.66</v>
+        <v>97.23999999999999</v>
       </c>
       <c r="AD10" t="n">
-        <v>97.91</v>
+        <v>97.02</v>
       </c>
       <c r="AE10" t="n">
-        <v>97.08</v>
+        <v>96.84</v>
       </c>
       <c r="AF10" t="n">
-        <v>97.39</v>
+        <v>96.09</v>
       </c>
       <c r="AG10" t="n">
-        <v>97.23999999999999</v>
+        <v>96.45999999999999</v>
       </c>
       <c r="AH10" t="n">
-        <v>97.02</v>
+        <v>96.84999999999999</v>
       </c>
       <c r="AI10" t="n">
-        <v>96.84</v>
+        <v>94.37</v>
       </c>
       <c r="AJ10" t="n">
-        <v>96.09</v>
+        <v>95.37</v>
       </c>
       <c r="AK10" t="n">
-        <v>96.45999999999999</v>
+        <v>94.87</v>
       </c>
       <c r="AL10" t="n">
-        <v>96.84999999999999</v>
+        <v>98.37</v>
       </c>
       <c r="AM10" t="n">
-        <v>94.37</v>
+        <v>98.48</v>
       </c>
       <c r="AN10" t="n">
-        <v>95.37</v>
+        <v>97.94</v>
       </c>
       <c r="AO10" t="n">
-        <v>94.87</v>
-      </c>
-      <c r="AP10" t="n">
-        <v>94.3</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>93.18000000000001</v>
-      </c>
-      <c r="AR10" t="n">
-        <v>91.53</v>
-      </c>
-      <c r="AS10" t="n">
-        <v>92.34</v>
+        <v>98.20999999999999</v>
       </c>
     </row>
     <row r="11">
@@ -1922,112 +1794,100 @@
         <v>97.91</v>
       </c>
       <c r="J11" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
       </c>
       <c r="K11" t="n">
-        <v>98.06</v>
+        <v>98.05</v>
       </c>
       <c r="L11" t="n">
-        <v>97.73</v>
+        <v>97.63</v>
       </c>
       <c r="M11" t="n">
-        <v>97.90000000000001</v>
+        <v>97.84</v>
       </c>
       <c r="N11" t="n">
         <v>98.29000000000001</v>
       </c>
       <c r="O11" t="n">
+        <v>97.81</v>
+      </c>
+      <c r="P11" t="n">
+        <v>97.61</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>97.70999999999999</v>
+      </c>
+      <c r="R11" t="n">
+        <v>98.28</v>
+      </c>
+      <c r="S11" t="n">
+        <v>97.95999999999999</v>
+      </c>
+      <c r="T11" t="n">
+        <v>97.59999999999999</v>
+      </c>
+      <c r="U11" t="n">
         <v>97.78</v>
       </c>
-      <c r="P11" t="n">
-        <v>97.66</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>97.72</v>
-      </c>
-      <c r="R11" t="n">
-        <v>98.29000000000001</v>
-      </c>
-      <c r="S11" t="n">
-        <v>97.81</v>
-      </c>
-      <c r="T11" t="n">
-        <v>97.61</v>
-      </c>
-      <c r="U11" t="n">
-        <v>97.70999999999999</v>
-      </c>
       <c r="V11" t="n">
-        <v>98.28</v>
+        <v>98.06999999999999</v>
       </c>
       <c r="W11" t="n">
-        <v>97.95999999999999</v>
+        <v>97.23999999999999</v>
       </c>
       <c r="X11" t="n">
-        <v>97.59999999999999</v>
+        <v>97.29000000000001</v>
       </c>
       <c r="Y11" t="n">
-        <v>97.78</v>
+        <v>97.27</v>
       </c>
       <c r="Z11" t="n">
-        <v>98.06999999999999</v>
+        <v>97.91</v>
       </c>
       <c r="AA11" t="n">
-        <v>97.23999999999999</v>
+        <v>96.98999999999999</v>
       </c>
       <c r="AB11" t="n">
-        <v>97.29000000000001</v>
+        <v>97.2</v>
       </c>
       <c r="AC11" t="n">
-        <v>97.27</v>
+        <v>97.09</v>
       </c>
       <c r="AD11" t="n">
-        <v>97.91</v>
+        <v>97.02</v>
       </c>
       <c r="AE11" t="n">
-        <v>96.98999999999999</v>
+        <v>96.98</v>
       </c>
       <c r="AF11" t="n">
-        <v>97.2</v>
+        <v>95.06</v>
       </c>
       <c r="AG11" t="n">
-        <v>97.09</v>
+        <v>96.01000000000001</v>
       </c>
       <c r="AH11" t="n">
-        <v>97.02</v>
+        <v>96.84999999999999</v>
       </c>
       <c r="AI11" t="n">
-        <v>96.98</v>
+        <v>96.43000000000001</v>
       </c>
       <c r="AJ11" t="n">
-        <v>95.06</v>
+        <v>95.20999999999999</v>
       </c>
       <c r="AK11" t="n">
-        <v>96.01000000000001</v>
+        <v>95.81</v>
       </c>
       <c r="AL11" t="n">
-        <v>96.84999999999999</v>
+        <v>98.37</v>
       </c>
       <c r="AM11" t="n">
-        <v>96.43000000000001</v>
+        <v>98.16</v>
       </c>
       <c r="AN11" t="n">
-        <v>95.20999999999999</v>
+        <v>97.64</v>
       </c>
       <c r="AO11" t="n">
-        <v>95.81</v>
-      </c>
-      <c r="AP11" t="n">
-        <v>94.3</v>
-      </c>
-      <c r="AQ11" t="n">
-        <v>93.55</v>
-      </c>
-      <c r="AR11" t="n">
-        <v>91.78</v>
-      </c>
-      <c r="AS11" t="n">
-        <v>92.66</v>
+        <v>97.90000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -2228,26 +2088,6 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AP12" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AQ12" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AR12" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AS12" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -2447,26 +2287,6 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AP13" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AQ13" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AR13" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AS13" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -2515,16 +2335,16 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
       </c>
       <c r="K14" t="n">
         <v>98.36</v>
       </c>
       <c r="L14" t="n">
-        <v>98.34999999999999</v>
+        <v>98.36</v>
       </c>
       <c r="M14" t="n">
-        <v>98.34999999999999</v>
+        <v>98.36</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -2662,26 +2482,6 @@
         </is>
       </c>
       <c r="AO14" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AP14" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AQ14" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AR14" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AS14" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2757,7 +2557,7 @@
         <v>98.29000000000001</v>
       </c>
       <c r="O15" t="n">
-        <v>98.28</v>
+        <v>98.29000000000001</v>
       </c>
       <c r="P15" t="n">
         <v>98.27</v>
@@ -2881,26 +2681,6 @@
         </is>
       </c>
       <c r="AO15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AP15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AQ15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AR15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AS15" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2993,16 +2773,16 @@
         </is>
       </c>
       <c r="R16" t="n">
-        <v>98.29000000000001</v>
+        <v>98.28</v>
       </c>
       <c r="S16" t="n">
-        <v>98.29000000000001</v>
+        <v>98.28</v>
       </c>
       <c r="T16" t="n">
         <v>98.27</v>
       </c>
       <c r="U16" t="n">
-        <v>98.28</v>
+        <v>98.27</v>
       </c>
       <c r="V16" t="inlineStr">
         <is>
@@ -3100,26 +2880,6 @@
         </is>
       </c>
       <c r="AO16" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AP16" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AQ16" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AR16" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AS16" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -3232,16 +2992,16 @@
         </is>
       </c>
       <c r="V17" t="n">
-        <v>98.28</v>
+        <v>98.06999999999999</v>
       </c>
       <c r="W17" t="n">
-        <v>98.28</v>
+        <v>98.06</v>
       </c>
       <c r="X17" t="n">
-        <v>98.27</v>
+        <v>98.04000000000001</v>
       </c>
       <c r="Y17" t="n">
-        <v>98.27</v>
+        <v>98.05</v>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
@@ -3319,26 +3079,6 @@
         </is>
       </c>
       <c r="AO17" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AP17" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AQ17" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AR17" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AS17" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -3471,16 +3211,16 @@
         </is>
       </c>
       <c r="Z18" t="n">
-        <v>98.06999999999999</v>
+        <v>97.91</v>
       </c>
       <c r="AA18" t="n">
-        <v>98.06</v>
+        <v>97.90000000000001</v>
       </c>
       <c r="AB18" t="n">
-        <v>98.04000000000001</v>
+        <v>97.89</v>
       </c>
       <c r="AC18" t="n">
-        <v>98.05</v>
+        <v>97.90000000000001</v>
       </c>
       <c r="AD18" t="inlineStr">
         <is>
@@ -3538,26 +3278,6 @@
         </is>
       </c>
       <c r="AO18" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AP18" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AQ18" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AR18" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AS18" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -3710,16 +3430,16 @@
         </is>
       </c>
       <c r="AD19" t="n">
-        <v>97.91</v>
+        <v>97.02</v>
       </c>
       <c r="AE19" t="n">
-        <v>97.90000000000001</v>
+        <v>97.01000000000001</v>
       </c>
       <c r="AF19" t="n">
-        <v>97.89</v>
+        <v>96.98999999999999</v>
       </c>
       <c r="AG19" t="n">
-        <v>97.90000000000001</v>
+        <v>97</v>
       </c>
       <c r="AH19" t="inlineStr">
         <is>
@@ -3757,26 +3477,6 @@
         </is>
       </c>
       <c r="AO19" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AP19" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AQ19" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AR19" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AS19" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -3949,16 +3649,16 @@
         </is>
       </c>
       <c r="AH20" t="n">
-        <v>97.02</v>
+        <v>96.84999999999999</v>
       </c>
       <c r="AI20" t="n">
-        <v>97.01000000000001</v>
+        <v>96.81999999999999</v>
       </c>
       <c r="AJ20" t="n">
-        <v>96.98999999999999</v>
+        <v>96.81999999999999</v>
       </c>
       <c r="AK20" t="n">
-        <v>97</v>
+        <v>96.81999999999999</v>
       </c>
       <c r="AL20" t="inlineStr">
         <is>
@@ -3976,26 +3676,6 @@
         </is>
       </c>
       <c r="AO20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AP20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AQ20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AR20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AS20" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -4188,255 +3868,16 @@
         </is>
       </c>
       <c r="AL21" t="n">
-        <v>96.84999999999999</v>
+        <v>98.37</v>
       </c>
       <c r="AM21" t="n">
-        <v>96.81999999999999</v>
+        <v>98.37</v>
       </c>
       <c r="AN21" t="n">
-        <v>96.81999999999999</v>
+        <v>98.36</v>
       </c>
       <c r="AO21" t="n">
-        <v>96.81999999999999</v>
-      </c>
-      <c r="AP21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AQ21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AR21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AS21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>LBFGS_LS</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="T22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="V22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="W22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="X22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="Y22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="Z22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AA22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AB22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AC22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AD22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AE22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AF22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AG22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AH22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AI22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AJ22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AK22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AL22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AM22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AN22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AO22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="AP22" t="n">
-        <v>94.3</v>
-      </c>
-      <c r="AQ22" t="n">
-        <v>94.26000000000001</v>
-      </c>
-      <c r="AR22" t="n">
-        <v>94.23</v>
-      </c>
-      <c r="AS22" t="n">
-        <v>94.23</v>
+        <v>98.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>